<commit_message>
Updates to name and index.html
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3126E073-D282-4729-B45D-7036032B3434}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -634,22 +635,22 @@
     <t>TESTE</t>
   </si>
   <si>
-    <t>'?' + odkSurvey.getHashString('MADTRAIL')</t>
-  </si>
-  <si>
-    <t>MADTRAIL</t>
-  </si>
-  <si>
-    <t>MADtrail</t>
-  </si>
-  <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>MADtrial</t>
+  </si>
+  <si>
+    <t>MADTRIAL</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('MADTRIAL')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1012,24 +1013,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1040,24 +1041,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1077,7 +1078,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1085,7 +1086,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1093,7 +1094,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1101,7 +1102,7 @@
         <v>20190521</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1112,7 +1113,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>173</v>
       </c>
@@ -1123,7 +1124,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>197</v>
       </c>
@@ -1134,12 +1135,12 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="10"/>
     </row>
   </sheetData>
@@ -1148,22 +1149,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>174</v>
       </c>
@@ -1177,21 +1178,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>192</v>
       </c>
       <c r="B2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" t="s">
         <v>204</v>
       </c>
-      <c r="C2" t="s">
-        <v>205</v>
-      </c>
       <c r="D2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -1199,7 +1200,7 @@
         <v>202</v>
       </c>
       <c r="C3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D3" t="s">
         <v>202</v>
@@ -1211,25 +1212,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>176</v>
       </c>
@@ -1252,7 +1253,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>182</v>
       </c>
@@ -1260,7 +1261,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
         <v>184</v>
       </c>
@@ -1271,12 +1272,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>186</v>
       </c>
@@ -1284,24 +1285,24 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E9" t="s">
         <v>190</v>
@@ -1310,17 +1311,17 @@
         <v>191</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>201</v>
       </c>
@@ -1331,24 +1332,24 @@
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
     </row>
   </sheetData>
@@ -1357,7 +1358,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1365,14 +1366,14 @@
       <selection pane="bottomLeft" activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.81640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="56.1796875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="43.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="56.140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
@@ -1383,7 +1384,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -1394,7 +1395,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
@@ -1405,7 +1406,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -1416,7 +1417,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1427,7 +1428,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1438,7 +1439,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
@@ -1449,7 +1450,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -1460,7 +1461,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>30</v>
       </c>
@@ -1471,7 +1472,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -1482,7 +1483,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>36</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>39</v>
       </c>
@@ -1504,7 +1505,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>41</v>
       </c>
@@ -1515,7 +1516,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>43</v>
       </c>
@@ -1526,7 +1527,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>45</v>
       </c>
@@ -1537,7 +1538,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>47</v>
       </c>
@@ -1548,7 +1549,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>49</v>
       </c>
@@ -1559,7 +1560,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>51</v>
       </c>
@@ -1570,7 +1571,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>54</v>
       </c>
@@ -1581,7 +1582,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>57</v>
       </c>
@@ -1592,7 +1593,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>60</v>
       </c>
@@ -1603,7 +1604,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>63</v>
       </c>
@@ -1614,7 +1615,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>66</v>
       </c>
@@ -1625,7 +1626,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>69</v>
       </c>
@@ -1636,7 +1637,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>72</v>
       </c>
@@ -1647,7 +1648,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>75</v>
       </c>
@@ -1658,7 +1659,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>78</v>
       </c>
@@ -1669,13 +1670,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>81</v>
       </c>
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>82</v>
       </c>
@@ -1686,7 +1687,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>84</v>
       </c>
@@ -1697,7 +1698,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>87</v>
       </c>
@@ -1708,7 +1709,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>90</v>
       </c>
@@ -1719,7 +1720,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>93</v>
       </c>
@@ -1730,7 +1731,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>96</v>
       </c>
@@ -1741,14 +1742,14 @@
         <v>199</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>98</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>99</v>
       </c>
@@ -1759,7 +1760,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>102</v>
       </c>
@@ -1770,7 +1771,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>105</v>
       </c>
@@ -1781,7 +1782,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>108</v>
       </c>
@@ -1792,7 +1793,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>111</v>
       </c>
@@ -1803,7 +1804,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>114</v>
       </c>
@@ -1814,7 +1815,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>117</v>
       </c>
@@ -1825,7 +1826,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>120</v>
       </c>
@@ -1836,7 +1837,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>123</v>
       </c>
@@ -1847,7 +1848,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>126</v>
       </c>
@@ -1858,7 +1859,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>129</v>
       </c>
@@ -1869,7 +1870,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>132</v>
       </c>
@@ -1880,7 +1881,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>135</v>
       </c>
@@ -1891,7 +1892,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>138</v>
       </c>
@@ -1902,7 +1903,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>141</v>
       </c>
@@ -1913,7 +1914,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>144</v>
       </c>
@@ -1924,7 +1925,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>145</v>
       </c>
@@ -1935,7 +1936,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>148</v>
       </c>
@@ -1946,7 +1947,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>151</v>
       </c>
@@ -1957,7 +1958,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>154</v>
       </c>
@@ -1968,7 +1969,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>157</v>
       </c>
@@ -1979,7 +1980,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>160</v>
       </c>
@@ -1990,7 +1991,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>163</v>
       </c>

</xml_diff>